<commit_message>
:+1: added some read line tricks
</commit_message>
<xml_diff>
--- a/rotten_tomatoes/movie_list/movie_content.xlsx
+++ b/rotten_tomatoes/movie_list/movie_content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangyanzhen/Developer/GitHub/CISC3014-IR-and-WebSearch-Project/rotten_tomatoes/movie_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222C0EE0-E9F8-6547-AB2C-70C09DA630AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDCAFFA-995A-E741-9CF6-2A8F9E5F9B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="560" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,9 +610,6 @@
     <t>Host</t>
   </si>
   <si>
-    <t xml:space="preserve">                    Six friends accidentally invite the attention of a demonic presence during an online séance and begin noticing strange occurrences in their homes.                </t>
-  </si>
-  <si>
     <t>Teenage Mutant Ninja Turtles: Mutant Mayhem</t>
   </si>
   <si>
@@ -938,6 +935,10 @@
   </si>
   <si>
     <t xml:space="preserve">                    Alice and Jack are lucky to be living in the idealized community of Victory, the experimental company town housing the men who work for the top-secret Victory Project and their families. The 1950's societal optimism espoused by their CEO, Frank--equal parts corporate visionary and motivational life coach--anchors every aspect of daily life in the tight-knit desert utopia. While the husbands spend every day inside the Victory Project Headquarters, working on the "development of progressive materials," their wives--including Frank's elegant partner, Shelley--get to spend their time enjoying the beauty, luxury and debauchery of their community. Life is perfect, with every resident's needs met by the company. All they ask in return is discretion and unquestioning commitment to the Victory cause. But when cracks in her idyllic life begin to appear, exposing flashes of something much more sinister lurking beneath the attractive façade, Alice can't help questioning exactly what they're doing in Victory, and why. Just how much is Alice willing to lose to expose what's really going on in this paradise?                </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                    Six friends accidentally invite the attention of a demonic presence during an online séance and begin noticing strange occurrences in their homes.                </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1312,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1342,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1562,7 +1563,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1694,7 +1695,7 @@
         <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1892,7 +1893,7 @@
         <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2145,7 +2146,7 @@
         <v>186</v>
       </c>
       <c r="C75" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2189,436 +2190,436 @@
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>196</v>
+        <v>303</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B80" t="s">
         <v>34</v>
       </c>
       <c r="C80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>198</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
         <v>199</v>
-      </c>
-      <c r="B81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" t="s">
         <v>201</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>202</v>
-      </c>
-      <c r="C82" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" t="s">
         <v>204</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>205</v>
-      </c>
-      <c r="C83" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" t="s">
         <v>207</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>208</v>
-      </c>
-      <c r="C84" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B85" t="s">
         <v>150</v>
       </c>
       <c r="C85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>211</v>
+      </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
         <v>212</v>
-      </c>
-      <c r="B86" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
+        <v>213</v>
+      </c>
+      <c r="B87" t="s">
         <v>214</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>215</v>
-      </c>
-      <c r="C87" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>216</v>
+      </c>
+      <c r="B88" t="s">
         <v>217</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>218</v>
-      </c>
-      <c r="C88" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>219</v>
+      </c>
+      <c r="B89" t="s">
         <v>220</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>221</v>
-      </c>
-      <c r="C89" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B90" t="s">
         <v>171</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
+        <v>224</v>
+      </c>
+      <c r="B91" t="s">
         <v>225</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>226</v>
-      </c>
-      <c r="C91" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" t="s">
         <v>228</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>229</v>
-      </c>
-      <c r="C92" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>230</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" t="s">
         <v>231</v>
-      </c>
-      <c r="B93" t="s">
-        <v>9</v>
-      </c>
-      <c r="C93" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B94" t="s">
         <v>73</v>
       </c>
       <c r="C94" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>236</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s">
         <v>237</v>
-      </c>
-      <c r="B96" t="s">
-        <v>9</v>
-      </c>
-      <c r="C96" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
+        <v>238</v>
+      </c>
+      <c r="B97" t="s">
         <v>239</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>240</v>
-      </c>
-      <c r="C97" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
+        <v>241</v>
+      </c>
+      <c r="B98" t="s">
         <v>242</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>243</v>
-      </c>
-      <c r="C98" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
+        <v>244</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
         <v>245</v>
-      </c>
-      <c r="B99" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
+        <v>246</v>
+      </c>
+      <c r="B100" t="s">
         <v>247</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>248</v>
-      </c>
-      <c r="C100" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
+        <v>249</v>
+      </c>
+      <c r="B101" t="s">
         <v>250</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>251</v>
-      </c>
-      <c r="C101" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B102" t="s">
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
+        <v>253</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
         <v>254</v>
-      </c>
-      <c r="B103" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>255</v>
+      </c>
+      <c r="B104" t="s">
         <v>256</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>257</v>
-      </c>
-      <c r="C104" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
+        <v>258</v>
+      </c>
+      <c r="B105" t="s">
         <v>259</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>260</v>
-      </c>
-      <c r="C105" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B106" t="s">
         <v>99</v>
       </c>
       <c r="C106" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
+        <v>263</v>
+      </c>
+      <c r="B107" t="s">
         <v>264</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>265</v>
-      </c>
-      <c r="C107" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
+        <v>266</v>
+      </c>
+      <c r="B108" t="s">
         <v>267</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>268</v>
-      </c>
-      <c r="C108" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
+        <v>269</v>
+      </c>
+      <c r="B109" t="s">
         <v>270</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>271</v>
-      </c>
-      <c r="C109" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>272</v>
+      </c>
+      <c r="B110" t="s">
         <v>273</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>274</v>
-      </c>
-      <c r="C110" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
+        <v>275</v>
+      </c>
+      <c r="B111" t="s">
         <v>276</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>277</v>
-      </c>
-      <c r="C111" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
+        <v>278</v>
+      </c>
+      <c r="B112" t="s">
         <v>279</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>280</v>
-      </c>
-      <c r="C112" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>281</v>
+      </c>
+      <c r="B113" t="s">
         <v>282</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>283</v>
-      </c>
-      <c r="C113" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>284</v>
+      </c>
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" t="s">
         <v>285</v>
-      </c>
-      <c r="B114" t="s">
-        <v>9</v>
-      </c>
-      <c r="C114" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B115" t="s">
         <v>56</v>
       </c>
       <c r="C115" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>288</v>
+      </c>
+      <c r="B116" t="s">
         <v>289</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>290</v>
-      </c>
-      <c r="C116" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
+        <v>291</v>
+      </c>
+      <c r="B117" t="s">
         <v>292</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>293</v>
-      </c>
-      <c r="C117" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
+        <v>294</v>
+      </c>
+      <c r="B118" t="s">
         <v>295</v>
       </c>
-      <c r="B118" t="s">
-        <v>296</v>
-      </c>
       <c r="C118" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>